<commit_message>
update process and scripts
</commit_message>
<xml_diff>
--- a/scripts/data/info.xlsx
+++ b/scripts/data/info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>A. baumanii</t>
   </si>
@@ -212,10 +212,58 @@
     <t>Gram-positive bacteria</t>
   </si>
   <si>
-    <t>Neither truly Gram-negative nor Gram-positive</t>
-  </si>
-  <si>
     <t>Coagulase-negative Staphilococci</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Acetinobacter baumannii</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>Enterococcus faecium</t>
+  </si>
+  <si>
+    <t>Neisseria gonorrhoeae</t>
+  </si>
+  <si>
+    <t>Mycobacterium tuberculosis</t>
+  </si>
+  <si>
+    <t>Proteus mirabilis</t>
+  </si>
+  <si>
+    <t>Clostridium difficile</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>Streptococcus pneumoniae</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Neither Gram-negative nor Gram-positive</t>
+  </si>
+  <si>
+    <t>Cell wall</t>
+  </si>
+  <si>
+    <t>Protein synthesis</t>
+  </si>
+  <si>
+    <t>DNA synthesis</t>
+  </si>
+  <si>
+    <t>Metabolism</t>
   </si>
 </sst>
 </file>
@@ -559,10 +607,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,11 +626,14 @@
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,6 +646,9 @@
       <c r="C2" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -605,6 +660,9 @@
       <c r="C3" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -616,6 +674,9 @@
       <c r="C4" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -627,6 +688,9 @@
       <c r="C5" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -638,6 +702,9 @@
       <c r="C6" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -647,7 +714,10 @@
         <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,6 +730,9 @@
       <c r="C8" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -672,7 +745,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -685,6 +758,9 @@
       <c r="C10" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -696,6 +772,9 @@
       <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -707,6 +786,9 @@
       <c r="C12" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -718,6 +800,9 @@
       <c r="C13" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -729,174 +814,285 @@
       <c r="C14" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B21" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B22" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B24" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B26" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B28" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C28" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B29" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C29" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B30" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C30" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="B31" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B32" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C34" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>